<commit_message>
update NACE 64 labels in all economic calibration data
</commit_message>
<xml_diff>
--- a/data/EPNM/interim/calibration_data/ERMG_revenue_survey.xlsx
+++ b/data/EPNM/interim/calibration_data/ERMG_revenue_survey.xlsx
@@ -22,193 +22,193 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
-    <t xml:space="preserve">01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31-32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37-39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41-43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55-56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59-60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62-63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69-70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74-75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80-82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87-88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90-92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97-98</t>
+    <t xml:space="preserve">A01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B05-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C13-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31-32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E37-39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F41-43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I55-56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J59-60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J62-63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M69-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M74-75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N80-82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q87-88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R90-92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T97-98</t>
   </si>
   <si>
     <t xml:space="preserve">BE</t>
@@ -326,13 +326,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X65"/>
+  <dimension ref="A1:X81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="1" style="0" width="9.07"/>
   </cols>
@@ -3200,6 +3200,22 @@
         <v>-8</v>
       </c>
     </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Plot fit economic model (#378)
</commit_message>
<xml_diff>
--- a/data/EPNM/interim/calibration_data/ERMG_revenue_survey.xlsx
+++ b/data/EPNM/interim/calibration_data/ERMG_revenue_survey.xlsx
@@ -22,193 +22,193 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
-    <t xml:space="preserve">01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31-32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37-39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41-43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55-56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59-60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62-63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69-70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74-75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80-82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87-88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90-92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97-98</t>
+    <t xml:space="preserve">A01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B05-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C13-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31-32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E37-39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F41-43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I55-56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J59-60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J62-63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M69-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M74-75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N80-82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q87-88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R90-92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T97-98</t>
   </si>
   <si>
     <t xml:space="preserve">BE</t>
@@ -326,13 +326,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X65"/>
+  <dimension ref="A1:X81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="1" style="0" width="9.07"/>
   </cols>
@@ -3200,6 +3200,22 @@
         <v>-8</v>
       </c>
     </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>